<commit_message>
Import openpyxl and win32com now working
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>test2</t>
   </si>
   <si>
@@ -35,15 +32,26 @@
   <si>
     <t>test5</t>
   </si>
+  <si>
+    <t>supppyy@hotmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +74,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,29 +399,35 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Almost complete, bug testing left
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -102,10 +102,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,61 +439,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>34324</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>34324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="supppyy@hotmail.com"/>
-    <hyperlink ref="A2" r:id="rId2" display="supppyy@hotmail.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="supppyy@hotmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="supppyy@hotmail.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="supppyy@hotmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>